<commit_message>
Processed original dataset and population and scenario information.
</commit_message>
<xml_diff>
--- a/data/ARM-HH-survey/economic_activity_codes.xlsx
+++ b/data/ARM-HH-survey/economic_activity_codes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\CCDR-ARM\data\ARM-HH-survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C65646C-4A85-4196-A423-EE27A7032B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0F28BD-44DE-412F-BF51-F7FB9871BFD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{39D88D36-E4D1-4B21-8AFA-4139E8C5C66A}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="180">
-  <si>
-    <t>NA</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="184">
   <si>
     <t>Բուսաբուծություն ու անասնաբուծություն, որսորդություն և հարակ</t>
   </si>
@@ -317,9 +314,6 @@
     <t>Mining of coal and brown coal (lignite).</t>
   </si>
   <si>
-    <t>xtraction of crude oil and natural gas</t>
-  </si>
-  <si>
     <t>Mining of metal ore</t>
   </si>
   <si>
@@ -515,9 +509,6 @@
     <t>Travel agencies, tour operators</t>
   </si>
   <si>
-    <t>nsuring security and conducting investigations</t>
-  </si>
-  <si>
     <t>Building maintenance and landscaping activities</t>
   </si>
   <si>
@@ -576,6 +567,27 @@
   </si>
   <si>
     <t>economic_activity_code</t>
+  </si>
+  <si>
+    <t>Extraction of crude oil and natural gas</t>
+  </si>
+  <si>
+    <t>Ensuring security and conducting investigations</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Manufacturing</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>ea_shortname</t>
+  </si>
+  <si>
+    <t>ea_shortcode</t>
   </si>
 </sst>
 </file>
@@ -945,42 +957,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBA8A8C-6ED3-4E92-B543-349AE2949063}">
-  <dimension ref="A1:D90"/>
+  <dimension ref="A1:E90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>-9999</v>
+        <v>175</v>
+      </c>
+      <c r="D1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -988,10 +1014,16 @@
       <c r="C3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -999,10 +1031,16 @@
       <c r="C4" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1010,940 +1048,1444 @@
       <c r="C5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
         <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+      <c r="E21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="E23" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+      <c r="D34">
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="D35">
+        <v>3</v>
+      </c>
+      <c r="E35" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
         <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
         <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
         <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="D39">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B40" t="s">
         <v>38</v>
       </c>
       <c r="C40" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="D40">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
         <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="D41">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B42" t="s">
         <v>40</v>
       </c>
       <c r="C42" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="D42">
+        <v>3</v>
+      </c>
+      <c r="E42" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B43" t="s">
         <v>41</v>
       </c>
       <c r="C43" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B44" t="s">
         <v>42</v>
       </c>
       <c r="C44" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
         <v>43</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+      <c r="E45" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
         <v>44</v>
       </c>
       <c r="C46" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+      <c r="E47" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
       </c>
       <c r="C48" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+      <c r="E48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
         <v>47</v>
       </c>
       <c r="C49" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B50" t="s">
         <v>48</v>
       </c>
       <c r="C50" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B51" t="s">
         <v>49</v>
       </c>
       <c r="C51" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="E51" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B52" t="s">
         <v>50</v>
       </c>
       <c r="C52" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+      <c r="E52" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B53" t="s">
         <v>51</v>
       </c>
       <c r="C53" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+      <c r="E53" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B54" t="s">
         <v>52</v>
       </c>
       <c r="C54" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+      <c r="E54" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B55" t="s">
         <v>53</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+      <c r="E55" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B56" t="s">
         <v>54</v>
       </c>
       <c r="C56" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+      <c r="E56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B57" t="s">
         <v>55</v>
       </c>
       <c r="C57" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+      <c r="E57" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
         <v>56</v>
       </c>
       <c r="C58" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B59" t="s">
         <v>57</v>
       </c>
       <c r="C59" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B60" t="s">
         <v>58</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+      <c r="E60" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B61" t="s">
         <v>59</v>
       </c>
       <c r="C61" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+      <c r="E61" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B62" t="s">
         <v>60</v>
       </c>
       <c r="C62" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+      <c r="E62" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B63" t="s">
         <v>61</v>
       </c>
       <c r="C63" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B64" t="s">
         <v>62</v>
       </c>
       <c r="C64" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+      <c r="E64" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B65" t="s">
         <v>63</v>
       </c>
       <c r="C65" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+      <c r="E65" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B66" t="s">
         <v>64</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+      <c r="E66" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B67" t="s">
         <v>65</v>
       </c>
       <c r="C67" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+      <c r="E67" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B68" t="s">
         <v>66</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B69" t="s">
         <v>67</v>
       </c>
       <c r="C69" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+      <c r="E69" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B70" t="s">
         <v>68</v>
       </c>
       <c r="C70" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+      <c r="E70" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B71" t="s">
         <v>69</v>
       </c>
       <c r="C71" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+      <c r="E71" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B72" t="s">
         <v>70</v>
       </c>
       <c r="C72" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+      <c r="E72" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B73" t="s">
         <v>71</v>
       </c>
-      <c r="D73" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>157</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B74" t="s">
         <v>72</v>
       </c>
       <c r="C74" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+      <c r="E74" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B75" t="s">
         <v>73</v>
       </c>
       <c r="C75" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+      <c r="E75" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B76" t="s">
         <v>74</v>
       </c>
       <c r="C76" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
+      <c r="E76" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B77" t="s">
         <v>75</v>
       </c>
       <c r="C77" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+      <c r="D77">
+        <v>3</v>
+      </c>
+      <c r="E77" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B78" t="s">
         <v>76</v>
       </c>
       <c r="C78" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+      <c r="E78" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B79" t="s">
         <v>77</v>
       </c>
       <c r="C79" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
+      <c r="E79" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B80" t="s">
         <v>78</v>
       </c>
       <c r="C80" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+      <c r="E80" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B81" t="s">
         <v>79</v>
       </c>
       <c r="C81" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+      <c r="D81">
+        <v>3</v>
+      </c>
+      <c r="E81" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B82" t="s">
         <v>80</v>
       </c>
       <c r="C82" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+      <c r="E82" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B83" t="s">
         <v>81</v>
       </c>
       <c r="C83" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B84" t="s">
         <v>82</v>
       </c>
       <c r="C84" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B85" t="s">
         <v>83</v>
       </c>
       <c r="C85" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="D85">
+        <v>3</v>
+      </c>
+      <c r="E85" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B86" t="s">
         <v>84</v>
       </c>
       <c r="C86" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="D86">
+        <v>3</v>
+      </c>
+      <c r="E86" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B87" t="s">
         <v>85</v>
       </c>
       <c r="C87" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="D87">
+        <v>3</v>
+      </c>
+      <c r="E87" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B88" t="s">
         <v>86</v>
       </c>
       <c r="C88" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>98</v>
+        <v>171</v>
+      </c>
+      <c r="D88">
+        <v>3</v>
+      </c>
+      <c r="E88" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>99</v>
       </c>
       <c r="B89" t="s">
         <v>87</v>
       </c>
       <c r="C89" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
-        <v>99</v>
-      </c>
-      <c r="B90" t="s">
-        <v>88</v>
-      </c>
-      <c r="C90" t="s">
-        <v>175</v>
+        <v>172</v>
+      </c>
+      <c r="D89">
+        <v>3</v>
+      </c>
+      <c r="E89" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>-9999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>